<commit_message>
20200517 1. X2範例EXCEL的收件者統編改回IL_GETNO 2. 併X3稅費合計Bug
</commit_message>
<xml_diff>
--- a/templates/(新報機單X2)轉出關貿格式範例.xlsx
+++ b/templates/(新報機單X2)轉出關貿格式範例.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Case\群翔\原始碼\20191209_Module\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F489C261-B8F1-4184-8D7C-E8A1073F4BC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE4EE1A-7E61-4E6E-8202-431B9B854BB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,10 +180,6 @@
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
   <si>
-    <t>${table:data.IL_GETNO_X2}</t>
-    <phoneticPr fontId="23" type="noConversion"/>
-  </si>
-  <si>
     <t>${table:data.IL_NEWSENDNAME_X2}</t>
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
@@ -227,6 +223,10 @@
     <t>${table:data.IL_TAXRATEEX}</t>
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
+  <si>
+    <t>${table:data.IL_GETNO}</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -262,33 +262,28 @@
       <sz val="11"/>
       <color indexed="9"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="52"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="9"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="10"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="52"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -300,7 +295,6 @@
       <sz val="18"/>
       <color indexed="56"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -313,77 +307,65 @@
       <sz val="11"/>
       <color indexed="63"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color indexed="56"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="20"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="60"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="62"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color indexed="23"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="15"/>
       <color indexed="56"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="17"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color indexed="56"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -401,7 +383,6 @@
       <b/>
       <sz val="12"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -1813,7 +1794,7 @@
         <v>34</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="34" t="s">
         <v>35</v>
@@ -1834,37 +1815,37 @@
         <v>40</v>
       </c>
       <c r="L5" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="M5" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="M5" s="40" t="s">
+      <c r="N5" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="N5" s="31" t="s">
+      <c r="O5" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="31" t="s">
+      <c r="P5" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q5" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="R5" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="P5" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q5" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="R5" s="71" t="s">
+      <c r="S5" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="43" t="s">
+      <c r="T5" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="44" t="s">
+      <c r="U5" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="U5" s="44" t="s">
+      <c r="V5" s="45" t="s">
         <v>48</v>
-      </c>
-      <c r="V5" s="45" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:27">

</xml_diff>